<commit_message>
Update plot with energy
</commit_message>
<xml_diff>
--- a/Lab3/file/sample_plot.xlsx
+++ b/Lab3/file/sample_plot.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>MIN-SEARCH</t>
   </si>
@@ -91,6 +91,9 @@
   <si>
     <t>V1 - V2 VARIATIONS</t>
   </si>
+  <si>
+    <t>ENERGY</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,43 +167,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -223,25 +189,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2481,6 +2449,37 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -2537,9 +2536,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$24:$F$24</c:f>
+              <c:f>Foglio1!$B$24:$G$24</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>POWER</c:v>
                 </c:pt>
@@ -2555,15 +2554,18 @@
                 <c:pt idx="4">
                   <c:v>EXE-TIME</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENERGY</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$B$25:$F$25</c:f>
+              <c:f>Foglio1!$B$25:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.37041610075319342</c:v>
                 </c:pt>
@@ -2578,6 +2580,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-272.72727272727275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-272.45787919945212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3194,6 +3199,37 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -3250,9 +3286,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$24:$F$24</c:f>
+              <c:f>Foglio1!$B$24:$G$24</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>POWER</c:v>
                 </c:pt>
@@ -3268,15 +3304,18 @@
                 <c:pt idx="4">
                   <c:v>EXE-TIME</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENERGY</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$B$26:$F$26</c:f>
+              <c:f>Foglio1!$B$26:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>36.552100381887712</c:v>
                 </c:pt>
@@ -3291,6 +3330,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-272.72727272727275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-246.14392699499072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6997,8 +7039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7013,11 +7055,11 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -7066,142 +7108,158 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="4">
         <v>32.396000000000001</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="4">
         <v>294197.8</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="4">
         <v>4.74</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="4">
         <v>131737</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>220</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4">
+        <f xml:space="preserve"> B7*F7</f>
+        <v>7127.12</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="4">
         <v>36.659999999999997</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="4">
         <v>281712.09999999998</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="4">
         <v>8.11</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="4">
         <v>112923</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>220</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4">
+        <f xml:space="preserve"> B8*F8</f>
+        <v>8065.1999999999989</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="4">
         <v>32.408000000000001</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="4">
         <v>294320.2</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="4">
         <v>4.88</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="4">
         <v>131807</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>160</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4">
+        <f xml:space="preserve"> B10*F10</f>
+        <v>5185.2800000000007</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="4">
         <v>38</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="4">
         <v>281994.59999999998</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="4">
         <v>6.27</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="4">
         <v>112929</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="11">
         <v>160</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4">
+        <f xml:space="preserve"> B11*F11</f>
+        <v>6080</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
@@ -7242,16 +7300,16 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="5"/>
@@ -7259,19 +7317,19 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="8">
         <f xml:space="preserve"> -(B7 - B8)*100/B7</f>
         <v>13.162118780096295</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <f t="shared" ref="B17:D17" si="0" xml:space="preserve"> -(C7 - C8)*100/C7</f>
         <v>-4.2439814301806509</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <f t="shared" si="0"/>
         <v>71.097046413502099</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
         <v>-14.281485080121758</v>
       </c>
@@ -7291,16 +7349,16 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="5"/>
@@ -7308,19 +7366,19 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="8">
         <f xml:space="preserve"> -(B10 - B11)*100/B10</f>
         <v>17.25499876573685</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="8">
         <f t="shared" ref="B20:D20" si="1" xml:space="preserve"> -(C10 - C11)*100/C10</f>
         <v>-4.1878199321691252</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <f t="shared" si="1"/>
         <v>28.483606557377044</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <f t="shared" si="1"/>
         <v>-14.322456318708415</v>
       </c>
@@ -7347,86 +7405,94 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="5"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="8">
         <f xml:space="preserve"> (B10 - B7)*1000/B7</f>
         <v>0.37041610075319342</v>
       </c>
-      <c r="C25" s="11">
-        <f t="shared" ref="C25:F26" si="2" xml:space="preserve"> (C10 - C7)*1000/C7</f>
+      <c r="C25" s="8">
+        <f t="shared" ref="C25:G26" si="2" xml:space="preserve"> (C10 - C7)*1000/C7</f>
         <v>0.41604661897547596</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <f t="shared" si="2"/>
         <v>29.535864978902886</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="8">
         <f t="shared" si="2"/>
         <v>0.5313617282919757</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="8">
         <f t="shared" si="2"/>
         <v>-272.72727272727275</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="8">
+        <f t="shared" si="2"/>
+        <v>-272.45787919945212</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="8">
         <f xml:space="preserve"> (B11 - B8)*1000/B8</f>
         <v>36.552100381887712</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="8">
         <f t="shared" ref="C26:E26" si="3" xml:space="preserve"> (C11 - C8)*1000/C8</f>
         <v>1.0027968269733534</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="8">
         <f t="shared" si="3"/>
         <v>-226.88039457459925</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="8">
         <f t="shared" si="3"/>
         <v>5.3133551180893177E-2</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="8">
         <f t="shared" si="2"/>
         <v>-272.72727272727275</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="8">
+        <f t="shared" si="2"/>
+        <v>-246.14392699499072</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
@@ -7435,7 +7501,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
@@ -7445,11 +7511,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A23:F23"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A23:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>